<commit_message>
Updated Marketing Tab of Formula for a Startup Workbook
</commit_message>
<xml_diff>
--- a/Spatial-Idea-Startup/Formula for a startup templates.xlsx
+++ b/Spatial-Idea-Startup/Formula for a startup templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharyzordo/Documents/Bootcamp GIS/Turn Your Spatial Idea Into a Successful Startup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F63DFA-52A3-BC40-995F-60DE04020F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D775C08-2D28-D843-95E8-90E1B8AF67C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="281">
   <si>
     <t>Define the MVP</t>
   </si>
@@ -112,12 +112,6 @@
   </si>
   <si>
     <t>Marketing Channels</t>
-  </si>
-  <si>
-    <t>Social - FB</t>
-  </si>
-  <si>
-    <t>Social - LinkedIn</t>
   </si>
   <si>
     <t>User Reach</t>
@@ -888,6 +882,15 @@
   </si>
   <si>
     <t>Helium Foundation</t>
+  </si>
+  <si>
+    <t>Social - FB - PPC</t>
+  </si>
+  <si>
+    <t>Social - LinkedIn - PPC</t>
+  </si>
+  <si>
+    <t>This is based on the sum of clicks determined in online and social ad spend, plus 5% of all other reach.</t>
   </si>
 </sst>
 </file>
@@ -1867,7 +1870,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1878,7 +1881,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
@@ -1889,7 +1892,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1900,7 +1903,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1911,7 +1914,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1922,7 +1925,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1953,7 +1956,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1961,7 +1964,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2001,7 +2004,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="22">
         <v>1466770</v>
@@ -2023,13 +2026,13 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>12</v>
@@ -2040,19 +2043,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D9" t="s">
-        <v>203</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>185</v>
-      </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2060,19 +2063,19 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2080,19 +2083,19 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" t="s">
         <v>195</v>
-      </c>
-      <c r="F11" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2100,19 +2103,19 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="E12" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>203</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="F12" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2120,19 +2123,19 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" t="s">
         <v>206</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="F13" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2140,21 +2143,21 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>198</v>
-      </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E25" s="21">
         <f>15000000000000/64000000000</f>
@@ -2163,7 +2166,7 @@
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26" s="20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E26" s="22">
         <v>350000</v>
@@ -2171,7 +2174,7 @@
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27" s="20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E27" s="8">
         <v>0.43</v>
@@ -2183,7 +2186,7 @@
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" s="20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E29" s="23">
         <f>E26/0.43</f>
@@ -2192,7 +2195,7 @@
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" s="20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E30" s="22">
         <v>1466770</v>
@@ -2200,7 +2203,7 @@
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D32" s="20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E32" s="3">
         <v>14000000000</v>
@@ -2208,7 +2211,7 @@
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E33" s="3">
         <f>E32/E30</f>
@@ -2247,7 +2250,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2277,10 +2280,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C4" s="5">
         <v>44774</v>
@@ -2291,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C5" s="5">
         <v>44804</v>
@@ -2302,7 +2305,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C6" s="5">
         <v>44804</v>
@@ -2313,7 +2316,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C7" s="5">
         <v>44804</v>
@@ -2324,7 +2327,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C8" s="5">
         <v>44834</v>
@@ -2335,7 +2338,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C9" s="5">
         <v>44834</v>
@@ -2346,7 +2349,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C10" s="5">
         <v>44880</v>
@@ -2357,7 +2360,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C11" s="5">
         <v>44895</v>
@@ -2368,7 +2371,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C12" s="5">
         <v>44957</v>
@@ -2379,14 +2382,14 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2399,13 +2402,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C15" s="5">
         <v>44788</v>
       </c>
       <c r="E15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -2414,7 +2417,7 @@
       </c>
       <c r="C16" s="5"/>
       <c r="E16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2423,7 +2426,7 @@
       </c>
       <c r="C17" s="5"/>
       <c r="E17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2432,7 +2435,7 @@
       </c>
       <c r="C18" s="5"/>
       <c r="E18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2440,13 +2443,13 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C19" s="5">
         <v>44788</v>
       </c>
       <c r="E19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2455,7 +2458,7 @@
       </c>
       <c r="C20" s="5"/>
       <c r="E20" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2464,7 +2467,7 @@
       </c>
       <c r="C21" s="5"/>
       <c r="E21" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2473,7 +2476,7 @@
       </c>
       <c r="C22" s="5"/>
       <c r="E22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2481,13 +2484,13 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C23" s="5">
         <v>44804</v>
       </c>
       <c r="E23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2496,7 +2499,7 @@
       </c>
       <c r="C24" s="5"/>
       <c r="E24" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2505,7 +2508,7 @@
       </c>
       <c r="C25" s="5"/>
       <c r="E25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2514,7 +2517,7 @@
       </c>
       <c r="C26" s="5"/>
       <c r="E26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -2522,13 +2525,13 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C27" s="5">
         <v>44804</v>
       </c>
       <c r="E27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2537,7 +2540,7 @@
       </c>
       <c r="C28" s="5"/>
       <c r="E28" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2546,7 +2549,7 @@
       </c>
       <c r="C29" s="5"/>
       <c r="E29" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2555,7 +2558,7 @@
       </c>
       <c r="C30" s="5"/>
       <c r="E30" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2563,13 +2566,13 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C31" s="5">
         <v>44834</v>
       </c>
       <c r="E31" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2578,7 +2581,7 @@
       </c>
       <c r="C32" s="5"/>
       <c r="E32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -2587,7 +2590,7 @@
       </c>
       <c r="C33" s="5"/>
       <c r="E33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -2596,7 +2599,7 @@
       </c>
       <c r="C34" s="5"/>
       <c r="E34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -2604,13 +2607,13 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C35" s="5">
         <v>44834</v>
       </c>
       <c r="E35" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -2619,7 +2622,7 @@
       </c>
       <c r="C36" s="5"/>
       <c r="E36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -2628,7 +2631,7 @@
       </c>
       <c r="C37" s="5"/>
       <c r="E37" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2637,7 +2640,7 @@
       </c>
       <c r="C38" s="5"/>
       <c r="E38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2645,13 +2648,13 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C39" s="5">
         <v>44880</v>
       </c>
       <c r="E39" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2660,7 +2663,7 @@
       </c>
       <c r="C40" s="5"/>
       <c r="E40" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2669,7 +2672,7 @@
       </c>
       <c r="C41" s="5"/>
       <c r="E41" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2678,7 +2681,7 @@
       </c>
       <c r="C42" s="5"/>
       <c r="E42" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2686,13 +2689,13 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C43" s="5">
         <v>44895</v>
       </c>
       <c r="E43" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2701,7 +2704,7 @@
       </c>
       <c r="C44" s="5"/>
       <c r="E44" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2710,7 +2713,7 @@
       </c>
       <c r="C45" s="5"/>
       <c r="E45" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2719,7 +2722,7 @@
       </c>
       <c r="C46" s="5"/>
       <c r="E46" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2727,13 +2730,13 @@
         <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C47" s="5">
         <v>44957</v>
       </c>
       <c r="E47" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2742,7 +2745,7 @@
       </c>
       <c r="C48" s="5"/>
       <c r="E48" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
@@ -2751,7 +2754,7 @@
       </c>
       <c r="C49" s="5"/>
       <c r="E49" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
@@ -2760,7 +2763,7 @@
       </c>
       <c r="C50" s="5"/>
       <c r="E50" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2787,7 +2790,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2802,7 +2805,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2819,139 +2822,139 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B3" s="28">
         <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B4" s="28">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B5" s="28">
         <v>0.36</v>
       </c>
       <c r="D5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B6" s="28">
         <v>10000</v>
       </c>
       <c r="D6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B7" s="16">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B8" s="16">
         <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B9" s="16">
         <v>3500</v>
       </c>
       <c r="D9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B10" s="16">
         <v>3.5</v>
       </c>
       <c r="D10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="N12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H13" s="17">
         <f>SUM($B$3*$B$7)</f>
@@ -2984,7 +2987,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H14" s="17">
         <f>SUM($B$4*$B$8)</f>
@@ -3017,7 +3020,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H15" s="17">
         <f>SUM($B$5*$B$9)</f>
@@ -3050,7 +3053,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H16" s="17">
         <f>SUM($B$6*$B$10)</f>
@@ -3083,7 +3086,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3134,7 +3137,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -3152,7 +3155,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3197,7 +3200,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3242,7 +3245,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22">
         <v>75</v>
@@ -3287,7 +3290,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D23">
         <v>4300</v>
@@ -3299,7 +3302,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B24">
         <f t="shared" ref="B24:M24" si="7">SUM(B20:B22)</f>
@@ -3374,7 +3377,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H27">
         <v>3200</v>
@@ -3386,7 +3389,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F28">
         <v>750</v>
@@ -3419,7 +3422,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -3472,7 +3475,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3490,7 +3493,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H32">
         <v>500</v>
@@ -3517,7 +3520,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G33">
         <v>3800</v>
@@ -3547,7 +3550,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D34">
         <v>4000</v>
@@ -3586,7 +3589,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G35">
         <v>3500</v>
@@ -3616,7 +3619,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B36">
         <f t="shared" ref="B36:G36" si="11">SUM(B32:B35)</f>
@@ -3673,7 +3676,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B38" s="14">
         <f>SUM(B17-B24-B29-B36)</f>
@@ -3730,17 +3733,17 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B42" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3757,7 +3760,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3789,11 +3792,11 @@
         <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -3806,7 +3809,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C4" s="6">
         <v>500</v>
@@ -3820,7 +3823,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C5" s="6">
         <v>120</v>
@@ -3834,7 +3837,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C6" s="6">
         <v>1000</v>
@@ -3843,7 +3846,7 @@
         <v>6000</v>
       </c>
       <c r="G6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -3851,7 +3854,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C7" s="6">
         <v>15800</v>
@@ -3860,7 +3863,7 @@
         <v>60000</v>
       </c>
       <c r="G7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -3868,7 +3871,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>278</v>
       </c>
       <c r="C8" s="6">
         <v>18900</v>
@@ -3877,7 +3880,7 @@
         <v>24000</v>
       </c>
       <c r="G8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -3885,7 +3888,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>279</v>
       </c>
       <c r="C9" s="6">
         <v>3000</v>
@@ -3894,12 +3897,12 @@
         <v>24000</v>
       </c>
       <c r="G9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6">
         <f>SUM(C4:C9)</f>
@@ -3915,7 +3918,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>16</v>
@@ -3933,7 +3936,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="7">
         <f>C10</f>
@@ -3945,14 +3948,18 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="7">
-        <f>SUM(C12*D13)</f>
-        <v>1966</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.05</v>
+        <f>SUM(C7:C9)+0.05*SUM(C4:C6)</f>
+        <v>37781</v>
+      </c>
+      <c r="D13" s="8" t="str">
+        <f>"---------------------------------------------------&gt;"</f>
+        <v>---------------------------------------------------&gt;</v>
+      </c>
+      <c r="G13" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -3960,11 +3967,11 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="7">
         <f t="shared" ref="C14:C16" si="0">SUM(C13*D14)</f>
-        <v>196.60000000000002</v>
+        <v>3778.1000000000004</v>
       </c>
       <c r="D14" s="8">
         <v>0.1</v>
@@ -3975,11 +3982,11 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="7">
         <f t="shared" si="0"/>
-        <v>19.660000000000004</v>
+        <v>377.81000000000006</v>
       </c>
       <c r="D15" s="8">
         <v>0.1</v>
@@ -3990,11 +3997,11 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="7">
         <f t="shared" si="0"/>
-        <v>1.9660000000000004</v>
+        <v>37.781000000000006</v>
       </c>
       <c r="D16" s="8">
         <v>0.1</v>
@@ -4080,7 +4087,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4095,13 +4102,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -4115,17 +4122,17 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -4133,23 +4140,23 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -4157,26 +4164,26 @@
         <v>3</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -4184,17 +4191,17 @@
         <v>4</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="9"/>
       <c r="C13" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -4202,40 +4209,40 @@
         <v>5</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C16" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
         <v>60</v>
-      </c>
-      <c r="D17" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -4263,7 +4270,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4278,16 +4285,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -4300,7 +4307,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -4308,25 +4315,25 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="10">
         <v>10000</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="10">
         <v>10000</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -4334,7 +4341,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -4342,37 +4349,37 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="10">
         <v>10000</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D9" s="10">
         <v>10000</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="10">
         <v>10000</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -4380,7 +4387,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -4388,13 +4395,13 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
       <c r="C12" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" s="10">
         <v>20000</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -4402,7 +4409,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
@@ -4410,13 +4417,13 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="9"/>
       <c r="C14" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D14" s="10">
         <v>5000</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -4424,7 +4431,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
@@ -4432,25 +4439,25 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D16" s="10">
         <v>20000</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="9"/>
       <c r="C17" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D17" s="10">
         <v>20000</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -4508,7 +4515,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4523,10 +4530,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -4541,10 +4548,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D4" s="9"/>
     </row>
@@ -4553,10 +4560,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D5" s="9"/>
     </row>
@@ -4565,10 +4572,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D6" s="9"/>
     </row>
@@ -4577,10 +4584,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D7" s="10"/>
     </row>
@@ -4589,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -4605,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
@@ -4615,7 +4622,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
@@ -4625,7 +4632,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
@@ -4635,7 +4642,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
@@ -4645,7 +4652,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -4655,7 +4662,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -4671,12 +4678,12 @@
         <v>1</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -4684,12 +4691,12 @@
         <v>2</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -4697,12 +4704,12 @@
         <v>3</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -4710,12 +4717,12 @@
         <v>4</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -4723,12 +4730,12 @@
         <v>5</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -4739,7 +4746,7 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -4797,7 +4804,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4809,7 +4816,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -4817,13 +4824,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -4837,13 +4844,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
@@ -4857,7 +4864,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="26"/>
@@ -4873,7 +4880,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="26"/>
@@ -4889,7 +4896,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="26"/>
@@ -4905,7 +4912,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="26"/>
@@ -4921,7 +4928,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="26"/>
@@ -4937,7 +4944,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="26"/>
@@ -4953,7 +4960,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="26"/>
@@ -4969,7 +4976,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="26"/>
@@ -4985,7 +4992,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="26"/>
@@ -5001,7 +5008,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="26"/>

</xml_diff>

<commit_message>
Update Financial Model Tab Based on Marketing Tab Updates
</commit_message>
<xml_diff>
--- a/Spatial-Idea-Startup/Formula for a startup templates.xlsx
+++ b/Spatial-Idea-Startup/Formula for a startup templates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharyzordo/Documents/Bootcamp GIS/Turn Your Spatial Idea Into a Successful Startup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D775C08-2D28-D843-95E8-90E1B8AF67C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8509BF-0C01-4448-8BF2-C847AB52D2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MVP" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="284">
   <si>
     <t>Define the MVP</t>
   </si>
@@ -530,9 +530,6 @@
   </si>
   <si>
     <t>Package 3 - Sales per mo</t>
-  </si>
-  <si>
-    <t>Website/SEO/Adwords</t>
   </si>
   <si>
     <t>Backlog</t>
@@ -854,12 +851,6 @@
     <t>Assumes 1 new implementation in month 1, and growth of 1 additional implementation month over month, for 21 implementations over 6 months)</t>
   </si>
   <si>
-    <t>ESRI User Conference (Including Lodging &amp; Airfare)</t>
-  </si>
-  <si>
-    <t>Web Mapping Services Monthly Margin Assumptions based on https://www.devicepilot.com/whitepapers/will-your-iot-product-make-a-profit</t>
-  </si>
-  <si>
     <t>ESRI User Conference Exhibitor</t>
   </si>
   <si>
@@ -891,6 +882,24 @@
   </si>
   <si>
     <t>This is based on the sum of clicks determined in online and social ad spend, plus 5% of all other reach.</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>ESRI User Conference Attendee (Including Lodging &amp; Airfare)</t>
+  </si>
+  <si>
+    <t>ESRI User Conference Exhibitor (including Lodging &amp; Airfare)</t>
+  </si>
+  <si>
+    <t>EnerGIS Conference Attendee</t>
+  </si>
+  <si>
+    <t>Website/SEO</t>
+  </si>
+  <si>
+    <t>Pay-Per-Click Advertising (Google AdWords, Facebook, LinkedIn)</t>
   </si>
 </sst>
 </file>
@@ -1870,7 +1879,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1881,7 +1890,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
@@ -1892,7 +1901,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1903,7 +1912,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1914,7 +1923,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -1925,7 +1934,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1964,7 +1973,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2004,7 +2013,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="22">
         <v>1466770</v>
@@ -2026,13 +2035,13 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>12</v>
@@ -2043,19 +2052,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E9" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" t="s">
         <v>183</v>
-      </c>
-      <c r="F9" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2063,19 +2072,19 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>186</v>
-      </c>
       <c r="F10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2083,19 +2092,19 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2103,19 +2112,19 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" t="s">
         <v>200</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" t="s">
         <v>202</v>
-      </c>
-      <c r="F12" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2123,19 +2132,19 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D13" t="s">
-        <v>201</v>
-      </c>
-      <c r="E13" s="13" t="s">
+      <c r="F13" t="s">
         <v>205</v>
-      </c>
-      <c r="F13" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2143,21 +2152,21 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" t="s">
         <v>196</v>
       </c>
-      <c r="D16" t="s">
-        <v>197</v>
-      </c>
       <c r="F16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E25" s="21">
         <f>15000000000000/64000000000</f>
@@ -2166,7 +2175,7 @@
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E26" s="22">
         <v>350000</v>
@@ -2174,7 +2183,7 @@
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E27" s="8">
         <v>0.43</v>
@@ -2186,7 +2195,7 @@
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E29" s="23">
         <f>E26/0.43</f>
@@ -2195,7 +2204,7 @@
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E30" s="22">
         <v>1466770</v>
@@ -2203,7 +2212,7 @@
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D32" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E32" s="3">
         <v>14000000000</v>
@@ -2211,7 +2220,7 @@
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E33" s="3">
         <f>E32/E30</f>
@@ -2250,7 +2259,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2280,10 +2289,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" t="s">
         <v>211</v>
-      </c>
-      <c r="B4" t="s">
-        <v>212</v>
       </c>
       <c r="C4" s="5">
         <v>44774</v>
@@ -2294,7 +2303,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C5" s="5">
         <v>44804</v>
@@ -2305,7 +2314,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C6" s="5">
         <v>44804</v>
@@ -2316,7 +2325,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C7" s="5">
         <v>44804</v>
@@ -2327,7 +2336,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C8" s="5">
         <v>44834</v>
@@ -2338,7 +2347,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C9" s="5">
         <v>44834</v>
@@ -2349,7 +2358,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C10" s="5">
         <v>44880</v>
@@ -2360,7 +2369,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C11" s="5">
         <v>44895</v>
@@ -2371,7 +2380,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C12" s="5">
         <v>44957</v>
@@ -2382,7 +2391,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>16</v>
@@ -2402,13 +2411,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C15" s="5">
         <v>44788</v>
       </c>
       <c r="E15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -2417,7 +2426,7 @@
       </c>
       <c r="C16" s="5"/>
       <c r="E16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2426,7 +2435,7 @@
       </c>
       <c r="C17" s="5"/>
       <c r="E17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2435,7 +2444,7 @@
       </c>
       <c r="C18" s="5"/>
       <c r="E18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2443,13 +2452,13 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C19" s="5">
         <v>44788</v>
       </c>
       <c r="E19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2458,7 +2467,7 @@
       </c>
       <c r="C20" s="5"/>
       <c r="E20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2467,7 +2476,7 @@
       </c>
       <c r="C21" s="5"/>
       <c r="E21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2476,7 +2485,7 @@
       </c>
       <c r="C22" s="5"/>
       <c r="E22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2484,13 +2493,13 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C23" s="5">
         <v>44804</v>
       </c>
       <c r="E23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2499,7 +2508,7 @@
       </c>
       <c r="C24" s="5"/>
       <c r="E24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2508,7 +2517,7 @@
       </c>
       <c r="C25" s="5"/>
       <c r="E25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2517,7 +2526,7 @@
       </c>
       <c r="C26" s="5"/>
       <c r="E26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -2525,13 +2534,13 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C27" s="5">
         <v>44804</v>
       </c>
       <c r="E27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2540,7 +2549,7 @@
       </c>
       <c r="C28" s="5"/>
       <c r="E28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2549,7 +2558,7 @@
       </c>
       <c r="C29" s="5"/>
       <c r="E29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2558,7 +2567,7 @@
       </c>
       <c r="C30" s="5"/>
       <c r="E30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2566,13 +2575,13 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C31" s="5">
         <v>44834</v>
       </c>
       <c r="E31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2581,7 +2590,7 @@
       </c>
       <c r="C32" s="5"/>
       <c r="E32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -2590,7 +2599,7 @@
       </c>
       <c r="C33" s="5"/>
       <c r="E33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -2599,7 +2608,7 @@
       </c>
       <c r="C34" s="5"/>
       <c r="E34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -2607,13 +2616,13 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C35" s="5">
         <v>44834</v>
       </c>
       <c r="E35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -2622,7 +2631,7 @@
       </c>
       <c r="C36" s="5"/>
       <c r="E36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -2631,7 +2640,7 @@
       </c>
       <c r="C37" s="5"/>
       <c r="E37" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2640,7 +2649,7 @@
       </c>
       <c r="C38" s="5"/>
       <c r="E38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2648,13 +2657,13 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C39" s="5">
         <v>44880</v>
       </c>
       <c r="E39" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2663,7 +2672,7 @@
       </c>
       <c r="C40" s="5"/>
       <c r="E40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2672,7 +2681,7 @@
       </c>
       <c r="C41" s="5"/>
       <c r="E41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2681,7 +2690,7 @@
       </c>
       <c r="C42" s="5"/>
       <c r="E42" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2689,13 +2698,13 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C43" s="5">
         <v>44895</v>
       </c>
       <c r="E43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2704,7 +2713,7 @@
       </c>
       <c r="C44" s="5"/>
       <c r="E44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2713,7 +2722,7 @@
       </c>
       <c r="C45" s="5"/>
       <c r="E45" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2722,7 +2731,7 @@
       </c>
       <c r="C46" s="5"/>
       <c r="E46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2730,13 +2739,13 @@
         <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C47" s="5">
         <v>44957</v>
       </c>
       <c r="E47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2745,7 +2754,7 @@
       </c>
       <c r="C48" s="5"/>
       <c r="E48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
@@ -2754,7 +2763,7 @@
       </c>
       <c r="C49" s="5"/>
       <c r="E49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
@@ -2763,7 +2772,7 @@
       </c>
       <c r="C50" s="5"/>
       <c r="E50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2774,10 +2783,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2822,46 +2831,46 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B3" s="28">
         <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="28">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B5" s="28">
         <v>0.36</v>
       </c>
       <c r="D5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B6" s="28">
         <v>10000</v>
       </c>
       <c r="D6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -2872,7 +2881,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -2883,7 +2892,7 @@
         <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -2894,18 +2903,18 @@
         <v>3500</v>
       </c>
       <c r="D9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B10" s="16">
         <v>3.5</v>
       </c>
       <c r="D10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -3053,7 +3062,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H16" s="17">
         <f>SUM($B$6*$B$10)</f>
@@ -3290,7 +3299,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D23">
         <v>4300</v>
@@ -3377,7 +3386,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="H27">
         <v>3200</v>
@@ -3389,366 +3398,424 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>162</v>
-      </c>
-      <c r="F28">
-        <v>750</v>
-      </c>
-      <c r="G28">
-        <v>400</v>
+        <v>280</v>
       </c>
       <c r="H28">
-        <v>400</v>
-      </c>
-      <c r="I28">
-        <v>400</v>
-      </c>
-      <c r="J28">
-        <v>400</v>
-      </c>
-      <c r="K28">
-        <v>400</v>
-      </c>
-      <c r="L28">
-        <v>400</v>
-      </c>
-      <c r="M28">
-        <v>400</v>
+        <v>7500</v>
       </c>
       <c r="N28">
         <f>SUM(B28:M28)</f>
-        <v>3550</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>281</v>
+      </c>
+      <c r="J29">
         <v>150</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <f>SUM(F27:F28)</f>
+      <c r="N29">
+        <f>SUM(B29:M29)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>282</v>
+      </c>
+      <c r="F30">
         <v>750</v>
       </c>
-      <c r="G29">
-        <f>SUM(G27:G28)</f>
+      <c r="G30">
         <v>400</v>
       </c>
-      <c r="H29">
-        <f t="shared" ref="H29:M29" si="8">SUM(H27:H28)</f>
-        <v>3600</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="8"/>
+      <c r="H30">
         <v>400</v>
       </c>
-      <c r="J29">
-        <f t="shared" si="8"/>
+      <c r="I30">
         <v>400</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="8"/>
+      <c r="J30">
         <v>400</v>
       </c>
-      <c r="L29">
-        <f t="shared" si="8"/>
+      <c r="K30">
         <v>400</v>
       </c>
-      <c r="M29">
-        <f t="shared" si="8"/>
+      <c r="L30">
         <v>400</v>
       </c>
-      <c r="N29">
-        <f t="shared" ref="N29" si="9">SUM(B29:M29)</f>
-        <v>6750</v>
+      <c r="M30">
+        <v>400</v>
+      </c>
+      <c r="N30">
+        <f>SUM(B30:M30)</f>
+        <v>3550</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="A31" t="s">
+        <v>283</v>
+      </c>
+      <c r="G31">
+        <v>9637.5</v>
+      </c>
+      <c r="H31">
+        <v>9637.5</v>
+      </c>
+      <c r="I31">
+        <v>9637.5</v>
+      </c>
+      <c r="J31">
+        <v>9637.5</v>
+      </c>
+      <c r="K31">
+        <v>9637.5</v>
+      </c>
+      <c r="L31">
+        <v>9637.5</v>
+      </c>
+      <c r="M31">
+        <v>9637.5</v>
+      </c>
+      <c r="N31">
+        <f>SUM(B31:M31)</f>
+        <v>67462.5</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>133</v>
+        <v>150</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ref="B32:L32" si="8">SUM(B27:B31)</f>
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="8"/>
+        <v>750</v>
+      </c>
+      <c r="G32">
+        <f>SUM(G27:G31)</f>
+        <v>10037.5</v>
       </c>
       <c r="H32">
-        <v>500</v>
+        <f>SUM(H27:H31)</f>
+        <v>20737.5</v>
       </c>
       <c r="I32">
-        <v>500</v>
+        <f>SUM(I27:I31)</f>
+        <v>10037.5</v>
       </c>
       <c r="J32">
-        <v>500</v>
+        <f>SUM(J27:J31)</f>
+        <v>10187.5</v>
       </c>
       <c r="K32">
-        <v>500</v>
+        <f>SUM(K27:K31)</f>
+        <v>10037.5</v>
       </c>
       <c r="L32">
-        <v>500</v>
+        <f>SUM(L27:L31)</f>
+        <v>10037.5</v>
       </c>
       <c r="M32">
-        <v>500</v>
+        <f>SUM(M27:M31)</f>
+        <v>10037.5</v>
       </c>
       <c r="N32">
         <f>SUM(B32:M32)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>262</v>
-      </c>
-      <c r="G33">
-        <v>3800</v>
-      </c>
-      <c r="H33">
-        <v>3800</v>
-      </c>
-      <c r="I33">
-        <v>3800</v>
-      </c>
-      <c r="J33">
-        <v>3800</v>
-      </c>
-      <c r="K33">
-        <v>3800</v>
-      </c>
-      <c r="L33">
-        <v>3800</v>
-      </c>
-      <c r="M33">
-        <v>3800</v>
-      </c>
-      <c r="N33">
-        <f>SUM(B33:M33)</f>
-        <v>26600</v>
+        <v>81862.5</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>134</v>
-      </c>
-      <c r="D34">
-        <v>4000</v>
-      </c>
-      <c r="E34">
-        <v>4000</v>
-      </c>
-      <c r="F34">
-        <v>4000</v>
-      </c>
-      <c r="G34">
-        <v>4000</v>
-      </c>
-      <c r="H34">
-        <v>4000</v>
-      </c>
-      <c r="I34">
-        <v>4000</v>
-      </c>
-      <c r="J34">
-        <v>4000</v>
-      </c>
-      <c r="K34">
-        <v>4000</v>
-      </c>
-      <c r="L34">
-        <v>4000</v>
-      </c>
-      <c r="M34">
-        <v>4000</v>
-      </c>
-      <c r="N34">
-        <f t="shared" ref="N34:N36" si="10">SUM(B34:M34)</f>
-        <v>40000</v>
-      </c>
+      <c r="A34" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>258</v>
-      </c>
-      <c r="G35">
-        <v>3500</v>
+        <v>133</v>
       </c>
       <c r="H35">
-        <v>3500</v>
+        <v>500</v>
       </c>
       <c r="I35">
-        <v>3500</v>
+        <v>500</v>
       </c>
       <c r="J35">
-        <v>3500</v>
+        <v>500</v>
       </c>
       <c r="K35">
-        <v>3500</v>
+        <v>500</v>
       </c>
       <c r="L35">
-        <v>3500</v>
+        <v>500</v>
       </c>
       <c r="M35">
-        <v>3500</v>
+        <v>500</v>
       </c>
       <c r="N35">
-        <f t="shared" si="10"/>
-        <v>24500</v>
+        <f>SUM(B35:M35)</f>
+        <v>3000</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>261</v>
+      </c>
+      <c r="G36">
+        <v>3800</v>
+      </c>
+      <c r="H36">
+        <v>3800</v>
+      </c>
+      <c r="I36">
+        <v>3800</v>
+      </c>
+      <c r="J36">
+        <v>3800</v>
+      </c>
+      <c r="K36">
+        <v>3800</v>
+      </c>
+      <c r="L36">
+        <v>3800</v>
+      </c>
+      <c r="M36">
+        <v>3800</v>
+      </c>
+      <c r="N36">
+        <f>SUM(B36:M36)</f>
+        <v>26600</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D37">
+        <v>4000</v>
+      </c>
+      <c r="E37">
+        <v>4000</v>
+      </c>
+      <c r="F37">
+        <v>4000</v>
+      </c>
+      <c r="G37">
+        <v>4000</v>
+      </c>
+      <c r="H37">
+        <v>4000</v>
+      </c>
+      <c r="I37">
+        <v>4000</v>
+      </c>
+      <c r="J37">
+        <v>4000</v>
+      </c>
+      <c r="K37">
+        <v>4000</v>
+      </c>
+      <c r="L37">
+        <v>4000</v>
+      </c>
+      <c r="M37">
+        <v>4000</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ref="N37:N39" si="9">SUM(B37:M37)</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>257</v>
+      </c>
+      <c r="G38">
+        <v>3500</v>
+      </c>
+      <c r="H38">
+        <v>3500</v>
+      </c>
+      <c r="I38">
+        <v>3500</v>
+      </c>
+      <c r="J38">
+        <v>3500</v>
+      </c>
+      <c r="K38">
+        <v>3500</v>
+      </c>
+      <c r="L38">
+        <v>3500</v>
+      </c>
+      <c r="M38">
+        <v>3500</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="9"/>
+        <v>24500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>150</v>
       </c>
-      <c r="B36">
-        <f t="shared" ref="B36:G36" si="11">SUM(B32:B35)</f>
+      <c r="B39">
+        <f t="shared" ref="B39:G39" si="10">SUM(B35:B38)</f>
         <v>0</v>
       </c>
-      <c r="C36">
+      <c r="C39">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="10"/>
+        <v>4000</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="10"/>
+        <v>4000</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="10"/>
+        <v>4000</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="10"/>
+        <v>11300</v>
+      </c>
+      <c r="H39">
+        <f>SUM(H35:H38)</f>
+        <v>11800</v>
+      </c>
+      <c r="I39">
+        <f t="shared" ref="I39:M39" si="11">SUM(I35:I38)</f>
+        <v>11800</v>
+      </c>
+      <c r="J39">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="D36">
+        <v>11800</v>
+      </c>
+      <c r="K39">
         <f t="shared" si="11"/>
-        <v>4000</v>
-      </c>
-      <c r="E36">
+        <v>11800</v>
+      </c>
+      <c r="L39">
         <f t="shared" si="11"/>
-        <v>4000</v>
-      </c>
-      <c r="F36">
+        <v>11800</v>
+      </c>
+      <c r="M39">
         <f t="shared" si="11"/>
-        <v>4000</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="11"/>
-        <v>11300</v>
-      </c>
-      <c r="H36">
-        <f>SUM(H32:H35)</f>
         <v>11800</v>
       </c>
-      <c r="I36">
-        <f t="shared" ref="I36:M36" si="12">SUM(I32:I35)</f>
-        <v>11800</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="12"/>
-        <v>11800</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="12"/>
-        <v>11800</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="12"/>
-        <v>11800</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="12"/>
-        <v>11800</v>
-      </c>
-      <c r="N36">
-        <f t="shared" si="10"/>
+      <c r="N39">
+        <f t="shared" si="9"/>
         <v>94100</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="14" t="s">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="14">
-        <f>SUM(B17-B24-B29-B36)</f>
+      <c r="B41" s="14">
+        <f>SUM(B17-B24-B32-B39)</f>
         <v>-75</v>
       </c>
-      <c r="C38" s="14">
-        <f>SUM(C17-C24-C29-C36)</f>
+      <c r="C41" s="14">
+        <f>SUM(C17-C24-C32-C39)</f>
         <v>-75</v>
       </c>
-      <c r="D38" s="14">
-        <f>SUM(D17-D24-D29-D36)</f>
+      <c r="D41" s="14">
+        <f>SUM(D17-D24-D32-D39)</f>
         <v>-10375</v>
       </c>
-      <c r="E38" s="14">
-        <f>SUM(E17-E24-E29-E36)</f>
+      <c r="E41" s="14">
+        <f>SUM(E17-E24-E32-E39)</f>
         <v>-6075</v>
       </c>
-      <c r="F38" s="14">
-        <f>SUM(F17-F24-F29-F36)</f>
+      <c r="F41" s="14">
+        <f>SUM(F17-F24-F32-F39)</f>
         <v>-6825</v>
       </c>
-      <c r="G38" s="14">
-        <f>SUM(G17-G24-G29-G36)</f>
-        <v>-13775</v>
-      </c>
-      <c r="H38" s="14">
-        <f>SUM(H17-H24-H29-H36)</f>
-        <v>20160</v>
-      </c>
-      <c r="I38" s="14">
-        <f>SUM(I17-I24-I29-I36)</f>
-        <v>23360</v>
-      </c>
-      <c r="J38" s="14">
-        <f>SUM(J17-J24-J29-J36)</f>
-        <v>23360</v>
-      </c>
-      <c r="K38" s="14">
-        <f>SUM(K17-K24-K29-K36)</f>
-        <v>23360</v>
-      </c>
-      <c r="L38" s="14">
-        <f>SUM(L17-L24-L29-L36)</f>
-        <v>23360</v>
-      </c>
-      <c r="M38" s="14">
-        <f>SUM(M17-M24-M29-M36)</f>
-        <v>23360</v>
-      </c>
-      <c r="N38" s="14">
-        <f>SUM(B38:M38)</f>
-        <v>99760</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="G41" s="14">
+        <f>SUM(G17-G24-G32-G39)</f>
+        <v>-23412.5</v>
+      </c>
+      <c r="H41" s="14">
+        <f>SUM(H17-H24-H32-H39)</f>
+        <v>3022.5</v>
+      </c>
+      <c r="I41" s="14">
+        <f>SUM(I17-I24-I32-I39)</f>
+        <v>13722.5</v>
+      </c>
+      <c r="J41" s="14">
+        <f>SUM(J17-J24-J32-J39)</f>
+        <v>13572.5</v>
+      </c>
+      <c r="K41" s="14">
+        <f>SUM(K17-K24-K32-K39)</f>
+        <v>13722.5</v>
+      </c>
+      <c r="L41" s="14">
+        <f>SUM(L17-L24-L32-L39)</f>
+        <v>13722.5</v>
+      </c>
+      <c r="M41" s="14">
+        <f>SUM(M17-M24-M32-M39)</f>
+        <v>13722.5</v>
+      </c>
+      <c r="N41" s="14">
+        <f>SUM(B41:M41)</f>
+        <v>24647.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="13" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B45" s="13" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B42" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B45" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -3759,8 +3826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3796,7 +3863,7 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -3809,7 +3876,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C4" s="6">
         <v>500</v>
@@ -3823,7 +3890,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C5" s="6">
         <v>120</v>
@@ -3837,16 +3904,16 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C6" s="6">
         <v>1000</v>
       </c>
       <c r="E6" s="18">
-        <v>6000</v>
+        <v>7500</v>
       </c>
       <c r="G6" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -3854,7 +3921,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C7" s="6">
         <v>15800</v>
@@ -3863,7 +3930,7 @@
         <v>60000</v>
       </c>
       <c r="G7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -3871,7 +3938,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C8" s="6">
         <v>18900</v>
@@ -3880,7 +3947,7 @@
         <v>24000</v>
       </c>
       <c r="G8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -3888,7 +3955,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C9" s="6">
         <v>3000</v>
@@ -3897,7 +3964,7 @@
         <v>24000</v>
       </c>
       <c r="G9" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -3910,7 +3977,7 @@
       </c>
       <c r="E10" s="18">
         <f>SUM(E4:E9)</f>
-        <v>114150</v>
+        <v>115650</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -3959,7 +4026,7 @@
         <v>---------------------------------------------------&gt;</v>
       </c>
       <c r="G13" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>